<commit_message>
Change '/' to '|'.
</commit_message>
<xml_diff>
--- a/docs/GraphuloFunctions.xlsx
+++ b/docs/GraphuloFunctions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="8850" windowHeight="6645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <t>1. Compute Jaccard on E by forming A = NoDiag(E.' * E)</t>
   </si>
   <si>
-    <t>2. NMF is doable on A, but doesn't make much sense.</t>
+    <t>** All are schema-dependent.</t>
   </si>
 </sst>
 </file>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,9 +470,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2">
-        <v>2</v>
-      </c>
+      <c r="C6" s="2"/>
       <c r="D6" t="s">
         <v>6</v>
       </c>
@@ -482,8 +480,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>